<commit_message>
pushing to the new repo
</commit_message>
<xml_diff>
--- a/Ebay/src/test/resources/userName_password.xlsx
+++ b/Ebay/src/test/resources/userName_password.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FinalFrameWorkTeam3\Ebay\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Final_Project_FrameWork\Ebay\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2364" windowHeight="228"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2364" windowHeight="228" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -36,6 +37,24 @@
   </si>
   <si>
     <t>Kisuar1234@</t>
+  </si>
+  <si>
+    <t>Pencil</t>
+  </si>
+  <si>
+    <t>Iphone</t>
+  </si>
+  <si>
+    <t>Toys</t>
+  </si>
+  <si>
+    <t>women's clothing</t>
+  </si>
+  <si>
+    <t>shoes</t>
+  </si>
+  <si>
+    <t>searchItem</t>
   </si>
 </sst>
 </file>
@@ -103,12 +122,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -394,7 +420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -428,4 +454,53 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>